<commit_message>
Dup KPI Dashboard Draft 01
First release of a Power BI dashboard draft for dupuytrens KPIs.
</commit_message>
<xml_diff>
--- a/Dupuytrens KPI.xlsx
+++ b/Dupuytrens KPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\Dupuytren-Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED7ADA2-EBF6-4222-8B5B-C4B12FEBB1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22F31D9-2559-405F-A1EE-62F8A867498E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26930" yWindow="4060" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phaseAggregates" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="115">
   <si>
     <t>Title</t>
   </si>
@@ -372,18 +372,44 @@
   <si>
     <t>[19] Comments</t>
   </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>SurveyName</t>
+  </si>
+  <si>
+    <t>PageName</t>
+  </si>
+  <si>
+    <t>QuestID</t>
+  </si>
+  <si>
+    <t>Dup88/questID (n=6659)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2017,7 +2043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="268">
+  <cellXfs count="272">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2286,6 +2312,10 @@
     <xf numFmtId="0" fontId="0" fillId="264" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="265" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="266" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2622,7 +2652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2827,7 +2857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -5026,7 +5058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y17" sqref="A17:Y18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8225,9 +8259,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:BA48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AG36" sqref="AG36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8255,10 +8291,12 @@
     <col min="22" max="22" width="34.6328125" customWidth="1"/>
     <col min="23" max="23" width="16.36328125" customWidth="1"/>
     <col min="24" max="24" width="14.08984375" customWidth="1"/>
-    <col min="25" max="25" width="13.6328125" customWidth="1"/>
+    <col min="25" max="27" width="13.6328125" customWidth="1"/>
+    <col min="31" max="31" width="10.54296875" customWidth="1"/>
+    <col min="32" max="32" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="3" t="s">
         <v>51</v>
       </c>
@@ -8325,8 +8363,52 @@
       <c r="W1" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB1" s="270" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC1" s="269" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD1" s="269" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE1" s="269" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF1" s="268" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG1" s="268"/>
+      <c r="AH1" s="268"/>
+      <c r="AI1" s="268"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="268" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="4"/>
+      <c r="AM1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
@@ -8396,8 +8478,66 @@
       <c r="W2">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB2" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC2" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD2" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF2" s="268" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG2" s="269"/>
+      <c r="AJ2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2">
+        <v>954</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM2">
+        <v>1229</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP2">
+        <v>1168</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS2">
+        <v>1184</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV2">
+        <v>1675</v>
+      </c>
+      <c r="AW2">
+        <v>1656</v>
+      </c>
+      <c r="AX2">
+        <v>1760</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA2">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -8467,8 +8607,66 @@
       <c r="W3">
         <v>751</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB3" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC3" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD3" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF3">
+        <v>88</v>
+      </c>
+      <c r="AG3" s="269"/>
+      <c r="AJ3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK3">
+        <v>783</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM3">
+        <v>1096</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP3">
+        <v>1052</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS3">
+        <v>1131</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV3">
+        <v>1573</v>
+      </c>
+      <c r="AW3">
+        <v>1604</v>
+      </c>
+      <c r="AX3">
+        <v>1641</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA3">
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -8538,8 +8736,126 @@
       <c r="W4">
         <v>1024</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB4" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC4" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD4" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF4">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="269"/>
+      <c r="AJ4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK4">
+        <v>776</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM4">
+        <v>1033</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP4">
+        <v>1000</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS4">
+        <v>1080</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV4">
+        <v>1505</v>
+      </c>
+      <c r="AW4">
+        <v>1558</v>
+      </c>
+      <c r="AX4">
+        <v>1523</v>
+      </c>
+      <c r="AZ4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA4">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB5" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC5" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD5" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF5">
+        <v>4</v>
+      </c>
+      <c r="AG5" s="269"/>
+      <c r="AJ5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK5">
+        <v>762</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM5">
+        <v>1026</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP5">
+        <v>995</v>
+      </c>
+      <c r="AR5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS5">
+        <v>1075</v>
+      </c>
+      <c r="AU5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV5">
+        <v>1407</v>
+      </c>
+      <c r="AW5">
+        <v>1548</v>
+      </c>
+      <c r="AX5">
+        <v>1510</v>
+      </c>
+      <c r="AZ5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA5">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>51</v>
       </c>
@@ -8609,8 +8925,66 @@
       <c r="X6" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB6" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC6" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD6" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF6">
+        <v>4</v>
+      </c>
+      <c r="AG6" s="269"/>
+      <c r="AJ6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK6">
+        <v>759</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM6">
+        <v>1026</v>
+      </c>
+      <c r="AO6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP6">
+        <v>992</v>
+      </c>
+      <c r="AR6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AS6">
+        <v>1074</v>
+      </c>
+      <c r="AU6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AV6">
+        <v>1406</v>
+      </c>
+      <c r="AW6">
+        <v>1548</v>
+      </c>
+      <c r="AX6">
+        <v>1511</v>
+      </c>
+      <c r="AZ6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="BA6">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
@@ -8683,8 +9057,126 @@
       <c r="X7">
         <v>990</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB7" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC7" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD7" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF7">
+        <v>4</v>
+      </c>
+      <c r="AG7" s="269"/>
+      <c r="AJ7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK7">
+        <v>757</v>
+      </c>
+      <c r="AL7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM7">
+        <v>1026</v>
+      </c>
+      <c r="AO7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP7">
+        <v>992</v>
+      </c>
+      <c r="AR7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS7">
+        <v>1073</v>
+      </c>
+      <c r="AU7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV7">
+        <v>1404</v>
+      </c>
+      <c r="AW7">
+        <v>1544</v>
+      </c>
+      <c r="AX7">
+        <v>1511</v>
+      </c>
+      <c r="AZ7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA7">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB8" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC8" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD8" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF8">
+        <v>4</v>
+      </c>
+      <c r="AG8" s="269"/>
+      <c r="AJ8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK8">
+        <v>756</v>
+      </c>
+      <c r="AL8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM8">
+        <v>1027</v>
+      </c>
+      <c r="AO8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP8">
+        <v>991</v>
+      </c>
+      <c r="AR8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS8">
+        <v>1074</v>
+      </c>
+      <c r="AU8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV8">
+        <v>1402</v>
+      </c>
+      <c r="AW8">
+        <v>1543</v>
+      </c>
+      <c r="AX8">
+        <v>1509</v>
+      </c>
+      <c r="AZ8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA8">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
         <v>51</v>
       </c>
@@ -8754,8 +9246,66 @@
       <c r="X9" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB9" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC9" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD9" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF9">
+        <v>4</v>
+      </c>
+      <c r="AG9" s="269"/>
+      <c r="AJ9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK9">
+        <v>755</v>
+      </c>
+      <c r="AL9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM9">
+        <v>1026</v>
+      </c>
+      <c r="AO9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP9">
+        <v>991</v>
+      </c>
+      <c r="AR9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS9">
+        <v>1074</v>
+      </c>
+      <c r="AU9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV9">
+        <v>1399</v>
+      </c>
+      <c r="AW9">
+        <v>1543</v>
+      </c>
+      <c r="AX9">
+        <v>1509</v>
+      </c>
+      <c r="AZ9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA9">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -8828,8 +9378,126 @@
       <c r="X10">
         <v>1070</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB10" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC10" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD10" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF10">
+        <v>4</v>
+      </c>
+      <c r="AG10" s="269"/>
+      <c r="AJ10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK10">
+        <v>755</v>
+      </c>
+      <c r="AL10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM10">
+        <v>1026</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP10">
+        <v>991</v>
+      </c>
+      <c r="AR10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS10">
+        <v>1073</v>
+      </c>
+      <c r="AU10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV10">
+        <v>1398</v>
+      </c>
+      <c r="AW10">
+        <v>1542</v>
+      </c>
+      <c r="AX10">
+        <v>1510</v>
+      </c>
+      <c r="AZ10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA10">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB11" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC11" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD11" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF11">
+        <v>3</v>
+      </c>
+      <c r="AG11" s="269"/>
+      <c r="AJ11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK11">
+        <v>753</v>
+      </c>
+      <c r="AL11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM11">
+        <v>1026</v>
+      </c>
+      <c r="AO11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP11">
+        <v>991</v>
+      </c>
+      <c r="AR11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS11">
+        <v>1074</v>
+      </c>
+      <c r="AU11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV11">
+        <v>1398</v>
+      </c>
+      <c r="AW11">
+        <v>1541</v>
+      </c>
+      <c r="AX11">
+        <v>1509</v>
+      </c>
+      <c r="AZ11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="BA11">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="3" t="s">
         <v>51</v>
       </c>
@@ -8902,8 +9570,68 @@
       <c r="Y12" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z12" s="271"/>
+      <c r="AA12" s="271"/>
+      <c r="AB12" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC12" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD12" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF12">
+        <v>3</v>
+      </c>
+      <c r="AG12" s="269"/>
+      <c r="AJ12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK12">
+        <v>753</v>
+      </c>
+      <c r="AL12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM12">
+        <v>1026</v>
+      </c>
+      <c r="AO12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP12">
+        <v>990</v>
+      </c>
+      <c r="AR12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS12">
+        <v>1073</v>
+      </c>
+      <c r="AU12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV12">
+        <v>1400</v>
+      </c>
+      <c r="AW12">
+        <v>1541</v>
+      </c>
+      <c r="AX12">
+        <v>1509</v>
+      </c>
+      <c r="AZ12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA12">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -8979,8 +9707,66 @@
       <c r="Y13">
         <v>1394</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB13" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC13" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD13" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF13">
+        <v>3</v>
+      </c>
+      <c r="AG13" s="269"/>
+      <c r="AJ13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK13">
+        <v>753</v>
+      </c>
+      <c r="AL13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM13">
+        <v>1026</v>
+      </c>
+      <c r="AO13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP13">
+        <v>990</v>
+      </c>
+      <c r="AR13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS13">
+        <v>1073</v>
+      </c>
+      <c r="AU13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV13">
+        <v>1398</v>
+      </c>
+      <c r="AW13">
+        <v>1541</v>
+      </c>
+      <c r="AX13">
+        <v>1509</v>
+      </c>
+      <c r="AZ13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA13">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
@@ -9056,8 +9842,66 @@
       <c r="Y14">
         <v>1540</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB14" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC14" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD14" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF14">
+        <v>3</v>
+      </c>
+      <c r="AG14" s="269"/>
+      <c r="AJ14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK14">
+        <v>815</v>
+      </c>
+      <c r="AL14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM14">
+        <v>1026</v>
+      </c>
+      <c r="AO14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP14">
+        <v>990</v>
+      </c>
+      <c r="AR14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS14">
+        <v>1073</v>
+      </c>
+      <c r="AU14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AV14">
+        <v>1397</v>
+      </c>
+      <c r="AW14">
+        <v>1541</v>
+      </c>
+      <c r="AX14">
+        <v>1512</v>
+      </c>
+      <c r="AZ14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BA14">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
@@ -9133,8 +9977,126 @@
       <c r="Y15">
         <v>1504</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB15" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC15" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD15" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF15">
+        <v>78</v>
+      </c>
+      <c r="AG15" s="269"/>
+      <c r="AJ15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK15">
+        <v>754</v>
+      </c>
+      <c r="AL15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM15">
+        <v>1026</v>
+      </c>
+      <c r="AO15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP15">
+        <v>990</v>
+      </c>
+      <c r="AR15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS15">
+        <v>1073</v>
+      </c>
+      <c r="AU15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV15">
+        <v>1398</v>
+      </c>
+      <c r="AW15">
+        <v>1541</v>
+      </c>
+      <c r="AX15">
+        <v>1509</v>
+      </c>
+      <c r="AZ15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA15">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB16" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC16" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD16" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF16">
+        <v>3</v>
+      </c>
+      <c r="AG16" s="269"/>
+      <c r="AJ16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK16">
+        <v>754</v>
+      </c>
+      <c r="AL16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM16">
+        <v>1026</v>
+      </c>
+      <c r="AO16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP16">
+        <v>990</v>
+      </c>
+      <c r="AR16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS16">
+        <v>1073</v>
+      </c>
+      <c r="AU16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV16">
+        <v>1394</v>
+      </c>
+      <c r="AW16">
+        <v>1541</v>
+      </c>
+      <c r="AX16">
+        <v>1509</v>
+      </c>
+      <c r="AZ16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA16">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
@@ -9207,8 +10169,68 @@
       <c r="Y17" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z17" s="271"/>
+      <c r="AA17" s="271"/>
+      <c r="AB17" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC17" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD17" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF17">
+        <v>3</v>
+      </c>
+      <c r="AG17" s="269"/>
+      <c r="AJ17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK17">
+        <v>752</v>
+      </c>
+      <c r="AL17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM17">
+        <v>1026</v>
+      </c>
+      <c r="AO17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP17">
+        <v>990</v>
+      </c>
+      <c r="AR17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS17">
+        <v>1073</v>
+      </c>
+      <c r="AU17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV17">
+        <v>1394</v>
+      </c>
+      <c r="AW17">
+        <v>1542</v>
+      </c>
+      <c r="AX17">
+        <v>1508</v>
+      </c>
+      <c r="AZ17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA17">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -9284,6 +10306,840 @@
       <c r="Y18">
         <v>1801</v>
       </c>
+      <c r="AB18" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC18" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD18" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF18">
+        <v>3</v>
+      </c>
+      <c r="AG18" s="269"/>
+      <c r="AJ18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK18">
+        <v>752</v>
+      </c>
+      <c r="AL18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM18">
+        <v>1027</v>
+      </c>
+      <c r="AO18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP18">
+        <v>990</v>
+      </c>
+      <c r="AR18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS18">
+        <v>1071</v>
+      </c>
+      <c r="AU18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV18">
+        <v>1397</v>
+      </c>
+      <c r="AW18">
+        <v>1541</v>
+      </c>
+      <c r="AX18">
+        <v>1507</v>
+      </c>
+      <c r="AZ18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA18">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB19" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC19" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD19" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF19">
+        <v>2</v>
+      </c>
+      <c r="AG19" s="269"/>
+      <c r="AJ19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK19">
+        <v>752</v>
+      </c>
+      <c r="AL19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM19">
+        <v>1025</v>
+      </c>
+      <c r="AO19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP19">
+        <v>990</v>
+      </c>
+      <c r="AR19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS19">
+        <v>1070</v>
+      </c>
+      <c r="AU19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AV19">
+        <v>1395</v>
+      </c>
+      <c r="AW19">
+        <v>1541</v>
+      </c>
+      <c r="AX19">
+        <v>1506</v>
+      </c>
+      <c r="AZ19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="BA19">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB20" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC20" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD20" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF20">
+        <v>2</v>
+      </c>
+      <c r="AG20" s="269"/>
+      <c r="AJ20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK20">
+        <v>753</v>
+      </c>
+      <c r="AL20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM20">
+        <v>1024</v>
+      </c>
+      <c r="AO20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP20">
+        <v>991</v>
+      </c>
+      <c r="AR20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS20">
+        <v>1070</v>
+      </c>
+      <c r="AU20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV20">
+        <v>1397</v>
+      </c>
+      <c r="AW20">
+        <v>1541</v>
+      </c>
+      <c r="AX20">
+        <v>1503</v>
+      </c>
+      <c r="AZ20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA20">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB21" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC21" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD21" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF21">
+        <v>2</v>
+      </c>
+      <c r="AG21" s="269"/>
+      <c r="AJ21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK21">
+        <v>752</v>
+      </c>
+      <c r="AL21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM21">
+        <v>1024</v>
+      </c>
+      <c r="AO21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP21">
+        <v>990</v>
+      </c>
+      <c r="AR21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS21">
+        <v>1070</v>
+      </c>
+      <c r="AU21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV21">
+        <v>1394</v>
+      </c>
+      <c r="AW21">
+        <v>1541</v>
+      </c>
+      <c r="AX21">
+        <v>1503</v>
+      </c>
+      <c r="AZ21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BA21">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="22" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB22" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC22" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD22" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF22">
+        <v>2</v>
+      </c>
+      <c r="AG22" s="269"/>
+      <c r="AJ22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK22">
+        <v>3429</v>
+      </c>
+      <c r="AL22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM22">
+        <v>4173</v>
+      </c>
+      <c r="AO22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP22">
+        <v>989</v>
+      </c>
+      <c r="AR22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AS22">
+        <v>4292</v>
+      </c>
+      <c r="AU22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV22">
+        <v>1392</v>
+      </c>
+      <c r="AW22">
+        <v>1541</v>
+      </c>
+      <c r="AX22">
+        <v>1504</v>
+      </c>
+      <c r="AZ22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA22">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="23" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB23" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC23" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD23" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF23">
+        <v>265</v>
+      </c>
+      <c r="AG23" s="269"/>
+      <c r="AJ23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK23">
+        <v>751</v>
+      </c>
+      <c r="AL23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM23">
+        <v>1024</v>
+      </c>
+      <c r="AO23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AR23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS23">
+        <v>1070</v>
+      </c>
+      <c r="AU23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV23">
+        <v>5504</v>
+      </c>
+      <c r="AW23">
+        <v>5048</v>
+      </c>
+      <c r="AX23">
+        <v>5300</v>
+      </c>
+      <c r="AZ23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA23">
+        <v>5711</v>
+      </c>
+    </row>
+    <row r="24" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB24" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC24" s="269">
+        <v>88</v>
+      </c>
+      <c r="AD24" s="269">
+        <v>20250101</v>
+      </c>
+      <c r="AE24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF24">
+        <v>58</v>
+      </c>
+      <c r="AG24" s="269"/>
+      <c r="AO24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP24">
+        <v>990</v>
+      </c>
+      <c r="AR24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS24">
+        <v>1070</v>
+      </c>
+      <c r="AU24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AV24">
+        <v>1394</v>
+      </c>
+      <c r="AW24">
+        <v>1540</v>
+      </c>
+      <c r="AX24">
+        <v>1502</v>
+      </c>
+      <c r="AZ24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BA24">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="25" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB25" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC25" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD25" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF25" s="268" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AV25">
+        <v>1394</v>
+      </c>
+      <c r="AW25">
+        <v>1540</v>
+      </c>
+      <c r="AX25">
+        <v>1504</v>
+      </c>
+      <c r="AZ25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA25">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="26" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB26" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC26" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD26" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF26">
+        <v>954</v>
+      </c>
+      <c r="AG26" s="269"/>
+    </row>
+    <row r="27" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB27" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC27" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD27" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF27">
+        <v>783</v>
+      </c>
+      <c r="AG27" s="269"/>
+    </row>
+    <row r="28" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB28" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC28" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD28" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF28">
+        <v>776</v>
+      </c>
+      <c r="AG28" s="269"/>
+    </row>
+    <row r="29" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB29" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC29" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD29" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF29">
+        <v>762</v>
+      </c>
+      <c r="AG29" s="269"/>
+    </row>
+    <row r="30" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB30" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC30" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD30" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF30">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="31" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB31" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC31" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD31" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF31">
+        <v>757</v>
+      </c>
+      <c r="AG31" s="269"/>
+    </row>
+    <row r="32" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB32" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC32" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD32" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF32">
+        <v>756</v>
+      </c>
+      <c r="AG32" s="269"/>
+    </row>
+    <row r="33" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB33" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC33" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD33" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF33">
+        <v>755</v>
+      </c>
+      <c r="AG33" s="269"/>
+    </row>
+    <row r="34" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB34" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC34" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD34" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF34">
+        <v>755</v>
+      </c>
+      <c r="AG34" s="269"/>
+    </row>
+    <row r="35" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB35" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC35" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD35" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF35">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="36" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB36" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC36" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD36" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF36">
+        <v>753</v>
+      </c>
+      <c r="AG36" s="269"/>
+    </row>
+    <row r="37" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB37" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC37" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD37" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF37">
+        <v>753</v>
+      </c>
+      <c r="AG37" s="269"/>
+    </row>
+    <row r="38" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB38" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC38" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD38" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF38">
+        <v>815</v>
+      </c>
+      <c r="AG38" s="269"/>
+    </row>
+    <row r="39" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB39" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC39" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD39" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF39">
+        <v>754</v>
+      </c>
+      <c r="AG39" s="269"/>
+    </row>
+    <row r="40" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB40" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC40" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD40" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE40" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF40">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="41" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB41" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC41" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD41" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE41" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF41">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="42" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB42" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC42" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD42" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF42">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="43" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB43" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC43" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD43" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE43" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF43">
+        <v>752</v>
+      </c>
+      <c r="AG43" s="269"/>
+    </row>
+    <row r="44" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB44" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC44" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD44" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF44">
+        <v>753</v>
+      </c>
+      <c r="AG44" s="269"/>
+    </row>
+    <row r="45" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB45" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC45" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD45" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE45" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF45">
+        <v>752</v>
+      </c>
+      <c r="AG45" s="269"/>
+    </row>
+    <row r="46" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB46" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC46" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD46" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE46" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF46">
+        <v>3429</v>
+      </c>
+      <c r="AG46" s="269"/>
+    </row>
+    <row r="47" spans="28:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB47" s="269" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC47" s="269">
+        <v>87</v>
+      </c>
+      <c r="AD47" s="269">
+        <v>20240102</v>
+      </c>
+      <c r="AE47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF47">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="48" spans="28:33" x14ac:dyDescent="0.35">
+      <c r="AD48" s="269"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11424,7 +13280,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -19250,7 +21108,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -19445,7 +21305,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>